<commit_message>
Add User Input: W,A,S,D,0 to control the Snake
</commit_message>
<xml_diff>
--- a/Excel Map.xlsx
+++ b/Excel Map.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Heron\Desktop\My Documents\Faculdade\3º Semestre\AOC\Trabalho AOC - Snake\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" tabRatio="623"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,7 +123,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,9 +161,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,7 +198,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,7 +233,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -414,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ET210"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="CS72" sqref="CS72"/>
+    <sheetView tabSelected="1" topLeftCell="BC19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BL35" sqref="BL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16614,7 +16609,7 @@
         <f t="shared" si="55"/>
         <v>16128</v>
       </c>
-      <c r="BN32" s="6">
+      <c r="BN32" s="3">
         <f t="shared" si="56"/>
         <v>16132</v>
       </c>

</xml_diff>